<commit_message>
stichprobe Signed-off-by: Mirko Matošin <mirko.matosin@hotmail.do>
</commit_message>
<xml_diff>
--- a/stichprobe.xlsx
+++ b/stichprobe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirko\PycharmProjects\ss22_dfss_clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4483DAD2-9BCF-485E-AE9A-F41FB2F71E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{82185901-1FE6-4318-B387-AA4385D9292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="-120" windowWidth="26490" windowHeight="16440" activeTab="1" xr2:uid="{C5D9D903-59D4-4798-9D75-07EE29993AE1}"/>
   </bookViews>
@@ -241,168 +241,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -422,6 +260,186 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -498,204 +516,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -715,6 +535,186 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -734,78 +734,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -825,6 +753,78 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -863,61 +863,61 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2743,70 +2743,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C10F2775-2B85-4B0D-B416-98D08454A0DC}" name="Tabelle1" displayName="Tabelle1" ref="A1:J14" totalsRowCount="1" headerRowDxfId="35" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C10F2775-2B85-4B0D-B416-98D08454A0DC}" name="Tabelle1" displayName="Tabelle1" ref="A1:J14" totalsRowCount="1" headerRowDxfId="36" dataDxfId="37">
   <autoFilter ref="A1:J13" xr:uid="{C10F2775-2B85-4B0D-B416-98D08454A0DC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J13">
     <sortCondition ref="J1:J13"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{39285984-2FD8-41D0-B341-4C397B8E3248}" name="Dateiname" totalsRowLabel="Ergebnis" dataDxfId="43" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{8FD303E2-168D-4B11-9C00-42966CADB051}" name="Tick_no" dataDxfId="42" totalsRowDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{32F98CD8-D31D-4C4E-A9E0-14EA51063638}" name="start" dataDxfId="41" totalsRowDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{AA1049DD-8E34-4EA7-9F63-B89CCD4F85E2}" name="ende" dataDxfId="40" totalsRowDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{632E267A-2AE1-4B4B-84EA-9C1A07BAFBA0}" name="tickdauer" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="20">
+    <tableColumn id="1" xr3:uid="{39285984-2FD8-41D0-B341-4C397B8E3248}" name="Dateiname" totalsRowLabel="Ergebnis" dataDxfId="43" totalsRowDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{8FD303E2-168D-4B11-9C00-42966CADB051}" name="Tick_no" dataDxfId="42" totalsRowDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{32F98CD8-D31D-4C4E-A9E0-14EA51063638}" name="start" dataDxfId="41" totalsRowDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{AA1049DD-8E34-4EA7-9F63-B89CCD4F85E2}" name="ende" dataDxfId="40" totalsRowDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{632E267A-2AE1-4B4B-84EA-9C1A07BAFBA0}" name="tickdauer" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="21">
       <calculatedColumnFormula>Tabelle1[[#This Row],[ende]]-Tabelle1[[#This Row],[start]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle1[tickdauer])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{205EF7AA-4EF4-43D1-A4EE-643A55BAA9D4}" name="maxFreq" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="19">
+    <tableColumn id="5" xr3:uid="{205EF7AA-4EF4-43D1-A4EE-643A55BAA9D4}" name="maxFreq" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="20">
       <totalsRowFormula>MEDIAN(Tabelle1[maxFreq])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{411BDD1A-82B2-4D57-A331-A0256F81A5FC}" name="maxTick" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="18">
+    <tableColumn id="6" xr3:uid="{411BDD1A-82B2-4D57-A331-A0256F81A5FC}" name="maxTick" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>MEDIAN(Tabelle1[maxTick])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{FA7BEC0F-86F0-42C8-A746-39F6C138AF97}" name="tickdavor" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="17">
+    <tableColumn id="10" xr3:uid="{FA7BEC0F-86F0-42C8-A746-39F6C138AF97}" name="tickdavor" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="19">
       <calculatedColumnFormula>Tabelle1[[#This Row],[maxTick]]-Tabelle1[[#This Row],[start]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle1[tickdavor])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5D020258-C33C-41F5-B6B2-128C2305FD67}" name="tickdanach" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="16">
+    <tableColumn id="9" xr3:uid="{5D020258-C33C-41F5-B6B2-128C2305FD67}" name="tickdanach" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="18">
       <calculatedColumnFormula>Tabelle1[[#This Row],[ende]]-Tabelle1[[#This Row],[maxTick]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle1[tickdanach])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{45219063-34B4-436F-81D9-18BCF712D174}" name="wandern" totalsRowFunction="count" dataDxfId="37" totalsRowDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{45219063-34B4-436F-81D9-18BCF712D174}" name="wandern" totalsRowFunction="count" dataDxfId="38" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42179411-9102-4DEC-9B91-41F038287E02}" name="Tabelle13" displayName="Tabelle13" ref="A18:J31" totalsRowCount="1" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{42179411-9102-4DEC-9B91-41F038287E02}" name="Tabelle13" displayName="Tabelle13" ref="A18:J31" totalsRowCount="1" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A18:J30" xr:uid="{42179411-9102-4DEC-9B91-41F038287E02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:J30">
     <sortCondition ref="J18:J30"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59607093-3D33-42AD-9ACA-1BAD5B375A8E}" name="Dateiname" totalsRowLabel="Ergebnis" dataDxfId="29" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{F4606A3A-67B5-4D1A-AD4C-1B1633566BFD}" name="Tick_no" dataDxfId="28" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{277B9CD6-D47E-46A7-B118-B03F1CF05DA4}" name="start" dataDxfId="27" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{D877A7C0-0E7E-48C5-B927-C1CEF617E015}" name="ende" dataDxfId="26" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{6CA664A7-0D1C-4842-9E26-F239DDA29442}" name="tickdauer" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="5">
+    <tableColumn id="1" xr3:uid="{59607093-3D33-42AD-9ACA-1BAD5B375A8E}" name="Dateiname" totalsRowLabel="Ergebnis" dataDxfId="30" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{F4606A3A-67B5-4D1A-AD4C-1B1633566BFD}" name="Tick_no" dataDxfId="29" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{277B9CD6-D47E-46A7-B118-B03F1CF05DA4}" name="start" dataDxfId="28" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D877A7C0-0E7E-48C5-B927-C1CEF617E015}" name="ende" dataDxfId="27" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6CA664A7-0D1C-4842-9E26-F239DDA29442}" name="tickdauer" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="7">
       <calculatedColumnFormula>Tabelle13[[#This Row],[ende]]-Tabelle13[[#This Row],[start]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle13[tickdauer])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{44E49D17-6E33-4584-9BF2-A17105F96107}" name="maxFreq" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{44E49D17-6E33-4584-9BF2-A17105F96107}" name="maxFreq" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="6">
       <totalsRowFormula>MEDIAN(Tabelle13[maxFreq])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{85D82B92-7304-4855-9B99-64FFE997F9A9}" name="maxTick" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="3">
+    <tableColumn id="6" xr3:uid="{85D82B92-7304-4855-9B99-64FFE997F9A9}" name="maxTick" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="5">
       <totalsRowFormula>MEDIAN(Tabelle13[maxTick])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{31026F88-3570-4813-8D8C-44CAD4430972}" name="tickdavor" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="2">
+    <tableColumn id="10" xr3:uid="{31026F88-3570-4813-8D8C-44CAD4430972}" name="tickdavor" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="4">
       <calculatedColumnFormula>Tabelle13[[#This Row],[maxTick]]-Tabelle13[[#This Row],[start]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle13[tickdavor])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06CDEE68-7236-4F51-8B17-B0C7808648D3}" name="tickdanach" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="9" xr3:uid="{06CDEE68-7236-4F51-8B17-B0C7808648D3}" name="tickdanach" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="3">
       <calculatedColumnFormula>Tabelle13[[#This Row],[ende]]-Tabelle13[[#This Row],[maxTick]]</calculatedColumnFormula>
       <totalsRowFormula>MEDIAN(Tabelle13[tickdanach])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F00F479D-A7E0-42F4-A593-5F3281AE2EFD}" name="wandern" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{F00F479D-A7E0-42F4-A593-5F3281AE2EFD}" name="wandern" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3203,13 +3203,15 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>